<commit_message>
Se modifica el diseño, fondo de pantalla, botones y se arregla el registro de docentes Se arregla el diseño de inicio de sesión
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Henao\Documents\Poryectos IntelliJ\ConexionU\src\main\resources\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3722B429-C45D-4233-BB0D-76BF361E5572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B24021-4B52-45A9-AA91-8713477C118A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
-    <sheet name="docentes" sheetId="1" r:id="rId1"/>
+    <sheet name="docentes" sheetId="5" r:id="rId1"/>
     <sheet name="estudiantes" sheetId="2" r:id="rId2"/>
     <sheet name="mentores" sheetId="3" r:id="rId3"/>
     <sheet name="notificaciones" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>Nombre</t>
   </si>
@@ -57,27 +57,6 @@
     <t>Receptor</t>
   </si>
   <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Henao</t>
-  </si>
-  <si>
-    <t>1018225388</t>
-  </si>
-  <si>
-    <t>dani23</t>
-  </si>
-  <si>
-    <t>daniel@elpoli.edu.com</t>
-  </si>
-  <si>
-    <t>3236547657</t>
-  </si>
-  <si>
-    <t>2004</t>
-  </si>
-  <si>
     <t>[Docente, Mentor, Estudiante]</t>
   </si>
   <si>
@@ -160,25 +139,61 @@
   </si>
   <si>
     <t>12345</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>juanp1</t>
+  </si>
+  <si>
+    <t>juan@gmail.com</t>
+  </si>
+  <si>
+    <t>3227322123</t>
+  </si>
+  <si>
+    <t>maryem</t>
+  </si>
+  <si>
+    <t>ruiz</t>
+  </si>
+  <si>
+    <t>maryem01</t>
+  </si>
+  <si>
+    <t>maryem01@gmail.com</t>
+  </si>
+  <si>
+    <t>3001234567</t>
+  </si>
+  <si>
+    <t>Docente</t>
+  </si>
+  <si>
+    <t>Antioquia</t>
+  </si>
+  <si>
+    <t>Medellín</t>
+  </si>
+  <si>
+    <t>El poli</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,20 +234,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,97 +556,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE4A813-3D5E-4C16-9A49-0750FE2BAD7F}">
-  <dimension ref="A1:K8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E67586-568B-45E9-BBD3-14C1735006BD}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="28.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.6640625"/>
-    <col min="8" max="8" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.0"/>
-    <col min="10" max="10" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.44140625"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E8" s="2"/>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -643,123 +642,158 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98190C0-1FD9-4C6C-A663-77BA4A6F0C62}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="24.33203125"/>
-    <col min="8" max="8" customWidth="true" width="12.44140625"/>
-    <col min="9" max="9" customWidth="true" width="15.44140625"/>
-    <col min="11" max="11" customWidth="true" width="12.44140625"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="F3" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="G3" t="s">
         <v>33</v>
       </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E4" t="s">
         <v>38</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F4" t="s">
         <v>39</v>
       </c>
-      <c r="G3" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>16</v>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -775,41 +809,41 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -825,9 +859,9 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Se crea en el esqueleto de la aplicación un nuevo botón para poder minimizar la ventana, aplica a la aplicación un ícono predeterminado Se cambian los mensajes que muestra la aplicación para que el ícono sea el mismo de la aplicación. En la ventana menú se crea un botón para cerrar sesión y se hacen cambios en cuanto al orden de los títulos.
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>Nombre</t>
   </si>
@@ -184,12 +184,34 @@
   </si>
   <si>
     <t>El poli</t>
+  </si>
+  <si>
+    <t>don</t>
+  </si>
+  <si>
+    <t>papaspapas</t>
+  </si>
+  <si>
+    <t>1032019684</t>
+  </si>
+  <si>
+    <t>donpapas35</t>
+  </si>
+  <si>
+    <t>donpapas35@salchipapas.com</t>
+  </si>
+  <si>
+    <t>3535353535</t>
+  </si>
+  <si>
+    <t>donpapa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -557,7 +579,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E67586-568B-45E9-BBD3-14C1735006BD}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K2"/>
@@ -601,37 +623,72 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="K3" t="s" s="0">
         <v>48</v>
       </c>
     </row>
@@ -650,10 +707,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="24.28515625"/>
+    <col min="8" max="8" customWidth="true" width="12.42578125"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125"/>
+    <col min="11" max="11" customWidth="true" width="12.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -692,107 +749,107 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se crea la primera version de la funcionalidad de ver la lista de los registros que hay en el archivo de excel a través de un tableview. Se cambia el nombre de la clase Dococente y queda con el nombre Usuario para que sea más general. Se hacen algunas correcciones a las validaciones del registro de nuevo usuario y queda pendiente arreglar cuando se ingresa un nuevo usuario en los campos de texto
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B24021-4B52-45A9-AA91-8713477C118A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B5D0E7-848C-4376-82FA-43A08E58CF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
   <si>
     <t>Nombre</t>
   </si>
@@ -205,6 +205,30 @@
   </si>
   <si>
     <t>donpapa</t>
+  </si>
+  <si>
+    <t>andres</t>
+  </si>
+  <si>
+    <t>lopez</t>
+  </si>
+  <si>
+    <t>1233445678</t>
+  </si>
+  <si>
+    <t>andres01</t>
+  </si>
+  <si>
+    <t>andres@gmail.com</t>
+  </si>
+  <si>
+    <t>P.C.J.I.C</t>
+  </si>
+  <si>
+    <t>1234567789</t>
+  </si>
+  <si>
+    <t>Estudiante</t>
   </si>
 </sst>
 </file>
@@ -579,9 +603,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E67586-568B-45E9-BBD3-14C1735006BD}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
@@ -657,7 +681,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
         <v>49</v>
       </c>
@@ -690,6 +714,41 @@
       </c>
       <c r="K3" t="s" s="0">
         <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -699,11 +758,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98190C0-1FD9-4C6C-A663-77BA4A6F0C62}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:K1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -851,6 +908,41 @@
       </c>
       <c r="K4" t="s" s="0">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="K5" t="s" s="0">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se crea la clase DataSingleton para que en ella se guarde la información con la cual el usuario inició sesión y desde la VentanaMenuController ya se puede acceder a esa información. Se establecen los estilos en el botón ingresar de la ventana-login y se cambian los colores del menú cuando el usuario inicia sesión como Estudiante. Se añaden imagenes de fondo verde.
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B5D0E7-848C-4376-82FA-43A08E58CF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10A65FF-FBC0-4F2B-AB44-CD85B3C76C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
   <si>
     <t>Nombre</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Receptor</t>
-  </si>
-  <si>
-    <t>[Docente, Mentor, Estudiante]</t>
   </si>
   <si>
     <t>[Antioquia, Caldas]</t>
@@ -235,7 +232,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -616,139 +612,139 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="F2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H2" t="s" s="0">
+      <c r="I2" t="s">
         <v>45</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="J2" t="s">
         <v>46</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="K2" t="s">
         <v>47</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="D3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="E3" t="s">
         <v>52</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="F3" t="s">
         <v>53</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="G3" t="s">
         <v>54</v>
       </c>
-      <c r="G3" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
         <v>45</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="J3" t="s">
         <v>46</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="K3" t="s">
         <v>47</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
         <v>56</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="C4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="D4" t="s">
         <v>58</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="E4" t="s">
         <v>59</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
         <v>60</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="K4" t="s" s="0">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -764,10 +760,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="24.28515625"/>
-    <col min="8" max="8" customWidth="true" width="12.42578125"/>
-    <col min="9" max="9" customWidth="true" width="15.42578125"/>
-    <col min="11" max="11" customWidth="true" width="12.42578125"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -775,174 +771,174 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="K2" t="s">
         <v>8</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="G3" t="s">
         <v>32</v>
       </c>
-      <c r="G3" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="K3" t="s">
         <v>8</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="C4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="D4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="E4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="F4" t="s">
         <v>38</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s" s="0">
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" t="s" s="0">
+      <c r="J4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="K4" t="s">
         <v>8</v>
       </c>
-      <c r="K4" t="s" s="0">
-        <v>9</v>
-      </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
         <v>62</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="E5" t="s" s="0">
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" t="s">
         <v>60</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>63</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="K5" t="s" s="0">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -965,34 +961,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se arreglan las opciones del menú cuando se inicia sesión como docente y estudiante para que se muestren de manera adecuada las ventanas. Se arregla la ventana-tableview para que muestre los registros correspondientes al tipo de usuario de inicia sesión
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10A65FF-FBC0-4F2B-AB44-CD85B3C76C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAF79DC-D104-44BB-9821-1AA4341BD374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
   <si>
     <t>Nombre</t>
   </si>
@@ -75,18 +75,12 @@
     <t>12672323</t>
   </si>
   <si>
-    <t>david12</t>
-  </si>
-  <si>
     <t>soto@elpoli.com</t>
   </si>
   <si>
     <t>8762346574</t>
   </si>
   <si>
-    <t>1234</t>
-  </si>
-  <si>
     <t>Apellido</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t>ruiz</t>
   </si>
   <si>
-    <t>maryem01</t>
-  </si>
-  <si>
     <t>maryem01@gmail.com</t>
   </si>
   <si>
@@ -226,6 +217,9 @@
   </si>
   <si>
     <t>Estudiante</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -601,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E67586-568B-45E9-BBD3-14C1735006BD}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,139 +606,139 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>43</v>
       </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>44</v>
-      </c>
-      <c r="I2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" t="s">
-        <v>54</v>
-      </c>
       <c r="H3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" t="s">
         <v>44</v>
-      </c>
-      <c r="I3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" t="s">
         <v>57</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -756,7 +750,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98190C0-1FD9-4C6C-A663-77BA4A6F0C62}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -771,34 +767,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -812,19 +808,19 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I2" t="s">
         <v>6</v>
@@ -838,28 +834,28 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I3" t="s">
         <v>6</v>
@@ -873,28 +869,28 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
         <v>6</v>
@@ -908,37 +904,37 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
         <v>55</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>56</v>
       </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
         <v>59</v>
       </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>62</v>
-      </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -961,34 +957,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Para el manejo de las asesorias nuevas se empiezan a registrar en datos/registros en una hoja nueva, de momento faltan las validaciones antes de ingresar una asesoría nueva. Se crea la clase Nodo y se cambia el nombre de la clase ListaDocentes a ListaNodos para manejar listas con nodos en el proyecto. Queda pendiente encontrar cómo usar los nodos en las listas actuales.
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAF79DC-D104-44BB-9821-1AA4341BD374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2BBBD5-28AF-4535-BB17-2D3C091AC0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
     <sheet name="estudiantes" sheetId="2" r:id="rId2"/>
     <sheet name="mentores" sheetId="3" r:id="rId3"/>
-    <sheet name="notificaciones" sheetId="4" r:id="rId4"/>
+    <sheet name="asesorias" sheetId="6" r:id="rId4"/>
+    <sheet name="notificaciones" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
   <si>
     <t>Nombre</t>
   </si>
@@ -220,6 +221,15 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Asesor</t>
+  </si>
+  <si>
+    <t>Motivo asesoría</t>
+  </si>
+  <si>
+    <t>Hora</t>
   </si>
 </sst>
 </file>
@@ -595,7 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E67586-568B-45E9-BBD3-14C1735006BD}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -993,6 +1003,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9274A02-017D-4EE9-9DE8-B2ADE117BFB2}">
   <dimension ref="A1:E1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Se agrega en la clase VentanaAsesoriasController un método para recuperar los datos del usuario que inició sesión. Esto con el fin de poder registrar en el archivo de excel los datos del Estudiante en la nueva asesoría agendada.
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2BBBD5-28AF-4535-BB17-2D3C091AC0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C080EB8-BBE6-4ADD-98B7-D9895B18410A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>Nombre</t>
   </si>
@@ -230,12 +230,28 @@
   </si>
   <si>
     <t>Hora</t>
+  </si>
+  <si>
+    <t>david soto</t>
+  </si>
+  <si>
+    <t>Maryem Ruíz</t>
+  </si>
+  <si>
+    <t>Consulta general</t>
+  </si>
+  <si>
+    <t>31-10-2023</t>
+  </si>
+  <si>
+    <t>00:20 - 00:40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -647,107 +663,107 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>57</v>
       </c>
     </row>
@@ -766,10 +782,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="24.28515625"/>
+    <col min="8" max="8" customWidth="true" width="12.42578125"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125"/>
+    <col min="11" max="11" customWidth="true" width="12.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -808,142 +824,142 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>57</v>
       </c>
     </row>
@@ -1004,17 +1020,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1039,6 +1053,23 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se aplica en la clase Asesoria un nuevo atributo de usuario para que se registre en el excel y de esta manera se pueda bsucar en el excel las asesorías y filtrar por usuario. Se hace la primera versión de la tabla para ver mis asesorías hechas.
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Henao\Documents\Poryectos IntelliJ\ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2BBBD5-28AF-4535-BB17-2D3C091AC0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB4312F-7E82-411E-BB76-534C67CBD381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
   <si>
     <t>Nombre</t>
   </si>
@@ -230,12 +230,28 @@
   </si>
   <si>
     <t>Hora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">david </t>
+  </si>
+  <si>
+    <t>Maryem Ruíz</t>
+  </si>
+  <si>
+    <t>Consulta tema de clase</t>
+  </si>
+  <si>
+    <t>30-11-2023</t>
+  </si>
+  <si>
+    <t>03:00 - 03:20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -609,9 +625,9 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -646,108 +662,108 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>57</v>
       </c>
     </row>
@@ -761,18 +777,18 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D12" sqref="D12:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="24.33203125"/>
+    <col min="8" max="8" customWidth="true" width="12.44140625"/>
+    <col min="9" max="9" customWidth="true" width="15.44140625"/>
+    <col min="11" max="11" customWidth="true" width="12.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -807,143 +823,143 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>57</v>
       </c>
     </row>
@@ -960,9 +976,9 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1004,41 +1020,63 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.44140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1053,9 +1091,9 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
se hace el ajuste de los perfiles para agendar asesoria quitando el super chanchullo que hizo nuestro amigo sebastian
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8804b01c0e612a3/Documentos/Proyectos_IntelliJ/PPI_ConexionU-master/PPI_ConexionU-master/src/main/resources/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C080EB8-BBE6-4ADD-98B7-D9895B18410A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2C080EB8-BBE6-4ADD-98B7-D9895B18410A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C58CC28-3FC3-46DD-B17B-6A4626D4E8B2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
   <si>
     <t>Nombre</t>
   </si>
@@ -245,13 +245,27 @@
   </si>
   <si>
     <t>00:20 - 00:40</t>
+  </si>
+  <si>
+    <t>Sebastian Palacio</t>
+  </si>
+  <si>
+    <t>Juan Carlos Gil</t>
+  </si>
+  <si>
+    <t>Consulta sobre módulos</t>
+  </si>
+  <si>
+    <t>07-11-2023</t>
+  </si>
+  <si>
+    <t>02:00 - 02:20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -625,9 +639,9 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -662,108 +676,108 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>60</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>60</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>41</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>42</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>43</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>49</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>50</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>51</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>41</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>42</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>43</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>52</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>55</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>56</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>40</v>
       </c>
-      <c r="G4" t="s" s="0">
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>41</v>
       </c>
-      <c r="I4" t="s" s="0">
+      <c r="I4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>43</v>
       </c>
-      <c r="K4" t="s" s="0">
+      <c r="K4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -776,19 +790,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98190C0-1FD9-4C6C-A663-77BA4A6F0C62}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="24.28515625"/>
-    <col min="8" max="8" customWidth="true" width="12.42578125"/>
-    <col min="9" max="9" customWidth="true" width="15.42578125"/>
-    <col min="11" max="11" customWidth="true" width="12.42578125"/>
+    <col min="5" max="5" width="24.26953125" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" customWidth="1"/>
+    <col min="11" max="11" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -823,143 +837,143 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>60</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>60</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>59</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>59</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>36</v>
       </c>
-      <c r="G4" t="s" s="0">
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>59</v>
       </c>
-      <c r="I4" t="s" s="0">
+      <c r="I4" t="s">
         <v>6</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>7</v>
       </c>
-      <c r="K4" t="s" s="0">
+      <c r="K4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>52</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>58</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>55</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>56</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" t="s" s="0">
+      <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>59</v>
       </c>
-      <c r="I5" t="s" s="0">
+      <c r="I5" t="s">
         <v>42</v>
       </c>
-      <c r="J5" t="s" s="0">
+      <c r="J5" t="s">
         <v>43</v>
       </c>
-      <c r="K5" t="s" s="0">
+      <c r="K5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -976,9 +990,9 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1020,18 +1034,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625"/>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>59</v>
       </c>
@@ -1054,21 +1071,38 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1084,9 +1118,9 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Se aplica la tabla del historial de las asesorias del estudiante
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Henao\Documents\Poryectos IntelliJ\ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="78">
   <si>
     <t>Nombre</t>
   </si>
@@ -245,12 +245,40 @@
   </si>
   <si>
     <t>03:00 - 03:20</t>
+  </si>
+  <si>
+    <t>Sebastian Palacio</t>
+  </si>
+  <si>
+    <t>Juan Carlos Gil</t>
+  </si>
+  <si>
+    <t>Consulta general</t>
+  </si>
+  <si>
+    <t>02-11-2023</t>
+  </si>
+  <si>
+    <t>02:20 - 02:40</t>
+  </si>
+  <si>
+    <t>Daniel Henao</t>
+  </si>
+  <si>
+    <t>Asesoría académica</t>
+  </si>
+  <si>
+    <t>25-11-2023</t>
+  </si>
+  <si>
+    <t>00:20 - 00:40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -662,107 +690,107 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>57</v>
       </c>
     </row>
@@ -781,10 +809,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="24.33203125"/>
+    <col min="8" max="8" customWidth="true" width="12.44140625"/>
+    <col min="9" max="9" customWidth="true" width="15.44140625"/>
+    <col min="11" max="11" customWidth="true" width="12.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -823,142 +851,142 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>57</v>
       </c>
     </row>
@@ -1019,7 +1047,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F3"/>
@@ -1027,9 +1055,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.44140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1058,23 +1086,63 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>68</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se hace commit para poder hacer merge con nueva_asesoria en github, es necesario hacer una clase AsesoriaTabla para solo infomación de la tabla
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Henao\Documents\Poryectos IntelliJ\ConexionU\src\main\resources\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F46705-F5B8-4BC8-A805-75BB163D9F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00456401-2B41-45F3-A2E8-F63F8623AD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
   <si>
     <t>Nombre</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>00:20 - 00:40</t>
+  </si>
+  <si>
+    <t>david soto</t>
+  </si>
+  <si>
+    <t>24-11-2023</t>
   </si>
 </sst>
 </file>
@@ -652,9 +658,9 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -689,7 +695,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
         <v>37</v>
       </c>
@@ -724,7 +730,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
         <v>45</v>
       </c>
@@ -759,7 +765,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="0">
         <v>52</v>
       </c>
@@ -807,15 +813,15 @@
       <selection activeCell="D12" sqref="D12:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="24.33203125"/>
-    <col min="8" max="8" customWidth="true" width="12.44140625"/>
-    <col min="9" max="9" customWidth="true" width="15.44140625"/>
-    <col min="11" max="11" customWidth="true" width="12.44140625"/>
+    <col min="5" max="5" customWidth="true" width="24.28515625"/>
+    <col min="8" max="8" customWidth="true" width="12.42578125"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125"/>
+    <col min="11" max="11" customWidth="true" width="12.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -850,7 +856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
         <v>9</v>
       </c>
@@ -885,7 +891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
         <v>24</v>
       </c>
@@ -920,7 +926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="0">
         <v>31</v>
       </c>
@@ -955,7 +961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s" s="0">
         <v>52</v>
       </c>
@@ -1003,9 +1009,9 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1047,20 +1053,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+      <selection activeCell="A5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.44140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.44140625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.109375"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>59</v>
       </c>
@@ -1085,7 +1091,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
         <v>64</v>
       </c>
@@ -1105,7 +1111,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
         <v>69</v>
       </c>
@@ -1125,7 +1131,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="0">
         <v>69</v>
       </c>
@@ -1142,6 +1148,26 @@
         <v>76</v>
       </c>
       <c r="F4" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s" s="0">
         <v>77</v>
       </c>
     </row>
@@ -1158,9 +1184,9 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Se deja lista la funcionalidad de cambiar la contraseña en la ventana-configuraciones, queda pendiente modificar el perfil
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>Nombre</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>02:00 - 02:20</t>
+  </si>
+  <si>
+    <t>12345</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Se configuran los archivos en carpetas para mayor organización y se crean las ventanas para las funcionalidades_menu/ventana-notificaciones y funcionalidades_menu/VentanaAgendasController
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Henao\Documents\Poryectos IntelliJ\ConexionU\src\main\resources\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4D1E74-29A5-4A81-AA08-E3EFC14540F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F4EFAE-82E0-42A2-B560-162D4982361B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
   <si>
     <t>Nombre</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>02:00 - 02:20</t>
+  </si>
+  <si>
+    <t>Fecha y hora</t>
   </si>
   <si>
     <t>12345</t>
@@ -594,17 +597,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E67586-568B-45E9-BBD3-14C1735006BD}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="27.109375"/>
-    <col min="12" max="12" customWidth="true" width="23.33203125"/>
+    <col min="5" max="5" customWidth="true" width="27.140625"/>
+    <col min="12" max="12" customWidth="true" width="23.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -642,7 +645,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
         <v>25</v>
       </c>
@@ -680,7 +683,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
         <v>38</v>
       </c>
@@ -731,15 +734,15 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="24.33203125"/>
-    <col min="8" max="8" customWidth="true" width="12.44140625"/>
-    <col min="9" max="9" customWidth="true" width="15.44140625"/>
-    <col min="11" max="11" customWidth="true" width="12.44140625"/>
+    <col min="5" max="5" customWidth="true" width="24.28515625"/>
+    <col min="8" max="8" customWidth="true" width="12.42578125"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125"/>
+    <col min="11" max="11" customWidth="true" width="12.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -774,7 +777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
         <v>32</v>
       </c>
@@ -822,9 +825,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -859,7 +862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
         <v>45</v>
       </c>
@@ -907,14 +910,14 @@
       <selection activeCell="F5" sqref="A2:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.44140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.44140625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.109375"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -939,7 +942,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
         <v>51</v>
       </c>
@@ -968,24 +971,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9274A02-017D-4EE9-9DE8-B2ADE117BFB2}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="12.0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Se cambian algunos fondos de pantalla de las funcionalidades de la aplicación, se cambian algunos diseños y se empieza a gestionar la lógica para recuperar el usuario del asesor en la funcionalidades_menu/ventana-asesorias
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8804b01c0e612a3/Documentos/Proyectos_IntelliJ/PPI_ConexionU-master/PPI_ConexionU-master/src/main/resources/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F4EFAE-82E0-42A2-B560-162D4982361B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{54F4EFAE-82E0-42A2-B560-162D4982361B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8033E652-3188-4CB8-9EA5-4E6FDDE3A2C2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>Nombre</t>
   </si>
@@ -193,32 +193,19 @@
     <t>Mentor</t>
   </si>
   <si>
-    <t>Daniel Henao</t>
-  </si>
-  <si>
-    <t>Maryem Ruiz</t>
-  </si>
-  <si>
-    <t>Consulta tema de clase</t>
-  </si>
-  <si>
-    <t>09-11-2023</t>
-  </si>
-  <si>
-    <t>02:00 - 02:20</t>
-  </si>
-  <si>
     <t>Fecha y hora</t>
   </si>
   <si>
-    <t>12345</t>
+    <t>Usuario Asesor</t>
+  </si>
+  <si>
+    <t>Usuario Estudiante</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -601,13 +588,13 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="27.140625"/>
-    <col min="12" max="12" customWidth="true" width="23.28515625"/>
+    <col min="5" max="5" width="27.1796875" customWidth="1"/>
+    <col min="12" max="12" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -645,79 +632,79 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>43</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" t="s" s="0">
+      <c r="L3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -734,15 +721,15 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="24.28515625"/>
-    <col min="8" max="8" customWidth="true" width="12.42578125"/>
-    <col min="9" max="9" customWidth="true" width="15.42578125"/>
-    <col min="11" max="11" customWidth="true" width="12.42578125"/>
+    <col min="5" max="5" width="24.26953125" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" customWidth="1"/>
+    <col min="11" max="11" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -777,38 +764,38 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -825,9 +812,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -862,38 +849,38 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -904,63 +891,45 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="A2:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625"/>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>55</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -971,19 +940,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9274A02-017D-4EE9-9DE8-B2ADE117BFB2}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="12.0"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Se arregla la manera en que se guardan las asesorías para que se puedan diferenciar por usuario, de tal manera que cada usuario tenga su asesoría asociada a su usuario. Se cambian los iconos de docente y estudiante, dependiendo de quién inicie sesión. Se aplica color al título de mis-asesorias para que cambie dependiendo de quien inicie sesión
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8804b01c0e612a3/Documentos/Proyectos_IntelliJ/PPI_ConexionU-master/PPI_ConexionU-master/src/main/resources/datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documents\Proyectos Intellij\PPI_ConexionU-menu\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{54F4EFAE-82E0-42A2-B560-162D4982361B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8033E652-3188-4CB8-9EA5-4E6FDDE3A2C2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0D6677-44E3-410F-8BDF-F31715EB4511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
   <si>
     <t>Nombre</t>
   </si>
@@ -200,6 +200,30 @@
   </si>
   <si>
     <t>Usuario Estudiante</t>
+  </si>
+  <si>
+    <t>Daniel Henao</t>
+  </si>
+  <si>
+    <t>Maryem Ruiz</t>
+  </si>
+  <si>
+    <t>Consulta general</t>
+  </si>
+  <si>
+    <t>11-11-2023</t>
+  </si>
+  <si>
+    <t>17:20 - 17:40</t>
+  </si>
+  <si>
+    <t>Emanuel Valencia</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>sss</t>
   </si>
 </sst>
 </file>
@@ -585,16 +609,16 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="27.1796875" customWidth="1"/>
-    <col min="12" max="12" width="23.26953125" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -632,7 +656,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -643,7 +667,7 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -670,7 +694,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -721,15 +745,15 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="24.26953125" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -764,7 +788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -809,12 +833,12 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -849,7 +873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -860,7 +884,7 @@
         <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
         <v>48</v>
@@ -891,20 +915,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -930,6 +955,52 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -942,12 +1013,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Se crea la clase AgendaSemanal para que se use en el guardado de agendas de manera semanal en el archivo de excel, en el cual se hace una nueva hoja para guardar estos datos.
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8804b01c0e612a3/Documentos/Proyectos_IntelliJ/PPI_ConexionU-master/PPI_ConexionU-master/src/main/resources/datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documents\Proyectos Intellij\PPI_ConexionU-menu\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{54F4EFAE-82E0-42A2-B560-162D4982361B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8033E652-3188-4CB8-9EA5-4E6FDDE3A2C2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AB6B7A-CC5C-4E46-B1B2-F349800A64F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" activeTab="4" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
     <sheet name="estudiantes" sheetId="2" r:id="rId2"/>
     <sheet name="mentores" sheetId="3" r:id="rId3"/>
     <sheet name="asesorias" sheetId="6" r:id="rId4"/>
-    <sheet name="notificaciones" sheetId="4" r:id="rId5"/>
+    <sheet name="Agendas" sheetId="7" r:id="rId5"/>
+    <sheet name="notificaciones" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>Nombre</t>
   </si>
@@ -200,6 +201,27 @@
   </si>
   <si>
     <t>Usuario Estudiante</t>
+  </si>
+  <si>
+    <t>Lunes</t>
+  </si>
+  <si>
+    <t>Martes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miércoles </t>
+  </si>
+  <si>
+    <t>Jueves</t>
+  </si>
+  <si>
+    <t>Viernes</t>
+  </si>
+  <si>
+    <t>Sábado</t>
+  </si>
+  <si>
+    <t>Domingo</t>
   </si>
 </sst>
 </file>
@@ -588,13 +610,13 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="27.1796875" customWidth="1"/>
-    <col min="12" max="12" width="23.26953125" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -632,7 +654,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -670,7 +692,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -721,15 +743,15 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="24.26953125" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -764,7 +786,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -812,9 +834,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -849,7 +871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -893,18 +915,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -937,17 +959,61 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0993C46-D7CC-4061-872F-039A4D5F145C}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9274A02-017D-4EE9-9DE8-B2ADE117BFB2}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Se añade en la ventana-mis-asesorias dos botones en la tabla de editar y eliminar asesoría, de momento no tienen validaciones.
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documents\Proyectos Intellij\PPI_ConexionU-menu\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AB6B7A-CC5C-4E46-B1B2-F349800A64F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7905839B-8D7A-465C-9195-21580E687DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" activeTab="4" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
   <si>
     <t>Nombre</t>
   </si>
@@ -222,12 +222,43 @@
   </si>
   <si>
     <t>Domingo</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>sss</t>
+  </si>
+  <si>
+    <t>Daniel Henao</t>
+  </si>
+  <si>
+    <t>David Rios</t>
+  </si>
+  <si>
+    <t>Asesoría PPI</t>
+  </si>
+  <si>
+    <t>15-11-2023</t>
+  </si>
+  <si>
+    <t>14:00 - 14:20</t>
+  </si>
+  <si>
+    <t>Maryem Ruiz</t>
+  </si>
+  <si>
+    <t>Consulta tema de clase</t>
+  </si>
+  <si>
+    <t>03:00 - 03:20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -607,13 +638,13 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="27.140625"/>
+    <col min="12" max="12" customWidth="true" width="23.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -655,78 +686,78 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>44</v>
       </c>
     </row>
@@ -740,15 +771,15 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="24.28515625"/>
+    <col min="8" max="8" customWidth="true" width="12.42578125"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125"/>
+    <col min="11" max="11" customWidth="true" width="12.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -787,37 +818,37 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -830,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182CF114-9740-44FA-A84D-C6C7B888094A}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,37 +903,37 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -913,17 +944,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125"/>
+    <col min="2" max="2" customWidth="true" width="18.140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -952,6 +981,52 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -962,12 +1037,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0993C46-D7CC-4061-872F-039A4D5F145C}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1010,7 +1085,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="12.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Hay una modificacion en la hoja de excel
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documents\Proyectos Intellij\PPI_ConexionU-menu\src\main\resources\datos\"/>
     </mc:Choice>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
   <si>
     <t>Nombre</t>
   </si>
@@ -222,12 +222,28 @@
   </si>
   <si>
     <t>Domingo</t>
+  </si>
+  <si>
+    <t>Daniel Henao</t>
+  </si>
+  <si>
+    <t>Maryem Ruiz</t>
+  </si>
+  <si>
+    <t>Consulta general</t>
+  </si>
+  <si>
+    <t>15-11-2023</t>
+  </si>
+  <si>
+    <t>06:20 - 06:40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -612,8 +628,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="27.140625"/>
+    <col min="12" max="12" customWidth="true" width="23.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -655,78 +671,78 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>44</v>
       </c>
     </row>
@@ -745,10 +761,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="24.28515625"/>
+    <col min="8" max="8" customWidth="true" width="12.42578125"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125"/>
+    <col min="11" max="11" customWidth="true" width="12.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -787,37 +803,37 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -872,37 +888,37 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -913,7 +929,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
@@ -921,9 +937,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125"/>
+    <col min="2" max="2" customWidth="true" width="18.140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -952,6 +968,29 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -966,8 +1005,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1010,7 +1049,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="12.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se hace una primera versión de un control de registros en excel para que un docente o mentor solo pueda dar un registro por día a la semana para dar asesorías a los estudiantes
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documents\Proyectos Intellij\PPI_ConexionU-menu\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AB6B7A-CC5C-4E46-B1B2-F349800A64F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8893E66B-7200-4802-B351-7E4F2531E501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" activeTab="4" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>Nombre</t>
   </si>
@@ -222,6 +222,42 @@
   </si>
   <si>
     <t>Domingo</t>
+  </si>
+  <si>
+    <t>Allison</t>
+  </si>
+  <si>
+    <t>Serna</t>
+  </si>
+  <si>
+    <t>1023629824</t>
+  </si>
+  <si>
+    <t>allis23</t>
+  </si>
+  <si>
+    <t>allisonserna@gmail.com</t>
+  </si>
+  <si>
+    <t>3044463002</t>
+  </si>
+  <si>
+    <t>allison</t>
+  </si>
+  <si>
+    <t>Allison Serna</t>
+  </si>
+  <si>
+    <t>Maryem Ruiz</t>
+  </si>
+  <si>
+    <t>Asesoría PPI</t>
+  </si>
+  <si>
+    <t>23-11-2023</t>
+  </si>
+  <si>
+    <t>02:40 - 03:00</t>
   </si>
 </sst>
 </file>
@@ -737,7 +773,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98190C0-1FD9-4C6C-A663-77BA4A6F0C62}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -818,6 +854,41 @@
         <v>17</v>
       </c>
       <c r="K2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -913,7 +984,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
@@ -952,6 +1023,29 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se arregla la manera en que se guardan las agendas disponibles desde el perfil de docente y mentor
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documents\Proyectos Intellij\PPI_ConexionU-menu\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8893E66B-7200-4802-B351-7E4F2531E501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD171917-5515-4D15-8CB3-BB1043310DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="97">
   <si>
     <t>Nombre</t>
   </si>
@@ -258,12 +258,85 @@
   </si>
   <si>
     <t>02:40 - 03:00</t>
+  </si>
+  <si>
+    <t>09:00-13:00</t>
+  </si>
+  <si>
+    <t>juandiego</t>
+  </si>
+  <si>
+    <t>mesa</t>
+  </si>
+  <si>
+    <t>1001469998</t>
+  </si>
+  <si>
+    <t>hades666</t>
+  </si>
+  <si>
+    <t>juandiegomesa234@gmaul.com</t>
+  </si>
+  <si>
+    <t>3226505292</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>Mel</t>
+  </si>
+  <si>
+    <t>Suarez</t>
+  </si>
+  <si>
+    <t>1011392080</t>
+  </si>
+  <si>
+    <t>Mel1227</t>
+  </si>
+  <si>
+    <t>mel@gmail.com</t>
+  </si>
+  <si>
+    <t>3205727115</t>
+  </si>
+  <si>
+    <t>Mel Suarez</t>
+  </si>
+  <si>
+    <t>02-12-2023</t>
+  </si>
+  <si>
+    <t>06:20 - 06:40</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>1000534371</t>
+  </si>
+  <si>
+    <t>john78tigre</t>
+  </si>
+  <si>
+    <t>john78tigres@gmail.com</t>
+  </si>
+  <si>
+    <t>3108929832</t>
+  </si>
+  <si>
+    <t>12345678</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -648,8 +721,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="27.140625"/>
+    <col min="12" max="12" customWidth="true" width="23.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -691,78 +764,78 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>44</v>
       </c>
     </row>
@@ -773,7 +846,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98190C0-1FD9-4C6C-A663-77BA4A6F0C62}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -781,10 +854,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="24.28515625"/>
+    <col min="8" max="8" customWidth="true" width="12.42578125"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125"/>
+    <col min="11" max="11" customWidth="true" width="12.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -823,72 +896,177 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -943,37 +1121,37 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -984,7 +1162,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
@@ -992,9 +1170,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125"/>
+    <col min="2" max="2" customWidth="true" width="18.140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1025,26 +1203,49 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>72</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1054,14 +1255,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0993C46-D7CC-4061-872F-039A4D5F145C}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1088,6 +1289,14 @@
       </c>
       <c r="H1" s="3" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1104,7 +1313,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="12.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se finaliza de arreglar la manera en que se guardan las agendas disponibles para la semana de asesorías, el calendario solo permite mostrar los días de la semana actual y que sean posteriores o iguales al día actual
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documents\Proyectos Intellij\PPI_ConexionU-menu\src\main\resources\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD171917-5515-4D15-8CB3-BB1043310DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6ECD192-CCCC-4898-A023-34446B9666A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="97">
   <si>
     <t>Nombre</t>
   </si>
@@ -260,9 +260,6 @@
     <t>02:40 - 03:00</t>
   </si>
   <si>
-    <t>09:00-13:00</t>
-  </si>
-  <si>
     <t>juandiego</t>
   </si>
   <si>
@@ -330,13 +327,15 @@
   </si>
   <si>
     <t>12345678</t>
+  </si>
+  <si>
+    <t>08:00 - 09:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -721,8 +720,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="27.140625"/>
-    <col min="12" max="12" customWidth="true" width="23.28515625"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -764,78 +763,78 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>43</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" t="s" s="0">
+      <c r="L3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -854,10 +853,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="24.28515625"/>
-    <col min="8" max="8" customWidth="true" width="12.42578125"/>
-    <col min="9" max="9" customWidth="true" width="15.42578125"/>
-    <col min="11" max="11" customWidth="true" width="12.42578125"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -896,177 +895,177 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>62</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>63</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>64</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>65</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>66</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>67</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
         <v>74</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="C4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="D4" t="s">
         <v>76</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="E4" t="s">
         <v>77</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="F4" t="s">
         <v>78</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="G4" t="s">
         <v>79</v>
       </c>
-      <c r="G4" t="s" s="0">
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>80</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="I4" t="s" s="0">
+      <c r="I5" t="s">
         <v>16</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J5" t="s">
         <v>17</v>
       </c>
-      <c r="K4" t="s" s="0">
+      <c r="K5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>81</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>83</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>85</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>86</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s" s="0">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" t="s">
         <v>19</v>
       </c>
-      <c r="I5" t="s" s="0">
+      <c r="I6" t="s">
         <v>16</v>
       </c>
-      <c r="J5" t="s" s="0">
+      <c r="J6" t="s">
         <v>17</v>
       </c>
-      <c r="K5" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>90</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>91</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>92</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>93</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>94</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>96</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K6" t="s" s="0">
+      <c r="K6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1121,37 +1120,37 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1170,9 +1169,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125"/>
-    <col min="2" max="2" customWidth="true" width="18.140625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1203,49 +1202,49 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>69</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>70</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>71</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
         <v>87</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>69</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="F3" t="s" s="0">
+      <c r="G3" t="s">
         <v>88</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1261,8 +1260,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.7109375"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1291,12 +1290,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>73</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1313,7 +1309,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="12.0"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se crea la primera version de la ventana-notificaciones con una tabla, se guarda en excel la información cuando se agrega una nueva asesoría, falta añadir la información a la tabla de la ventana
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/registros.xlsx
+++ b/src/main/resources/datos/registros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\Proyectos_IntelliJ\PPI_ConexionU\src\main\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9861194-0C0B-4B07-BF49-40E918374928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88505DF-D113-4939-976A-8D842A0C5397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{DFBFC2F8-E22A-4AB0-A134-807EA5721186}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="104">
   <si>
     <t>Nombre</t>
   </si>
@@ -327,6 +327,30 @@
   </si>
   <si>
     <t>12345678</t>
+  </si>
+  <si>
+    <t>Daniel Henao</t>
+  </si>
+  <si>
+    <t>Consulta general</t>
+  </si>
+  <si>
+    <t>03-12-2023</t>
+  </si>
+  <si>
+    <t>07:00 - 07:20</t>
+  </si>
+  <si>
+    <t>Nueva asesoría agendada</t>
+  </si>
+  <si>
+    <t>02-12-23 00:27</t>
+  </si>
+  <si>
+    <t>Danielnull</t>
+  </si>
+  <si>
+    <t>Se ha agendado una nueva asesoría, REVISAR EN MIS ASESORÍAS</t>
   </si>
 </sst>
 </file>
@@ -711,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E67586-568B-45E9-BBD3-14C1735006BD}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1158,7 +1182,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FF7F67-97C1-41B4-ABB5-EAC0278706AA}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
@@ -1242,6 +1266,29 @@
       </c>
       <c r="G3" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1295,13 +1342,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9274A02-017D-4EE9-9DE8-B2ADE117BFB2}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1321,6 +1371,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>